<commit_message>
updated project log, fixed spelling mistakes
</commit_message>
<xml_diff>
--- a/other-project-docs/Project Activity Log (Female Literacy).xlsx
+++ b/other-project-docs/Project Activity Log (Female Literacy).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalie/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6227A1BC-125E-9049-AB95-92C674C08B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB90C89-5B1E-2A49-86F6-F2786BA16C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,12 +39,39 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <scheme val="minor"/>
+            <family val="2"/>
           </rPr>
-          <t>======
-ID#AAAAwogVklY
-natalie feak    (2023-05-10 16:18:39)
-This was done within the class session, so doesn't count towards our minutes</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAAwogVklY
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">natalie feak    (2023-05-10 16:18:39)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This was done within the class session, so doesn't count towards our minutes</t>
         </r>
       </text>
     </comment>
@@ -58,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="130">
   <si>
     <t>Name:</t>
   </si>
@@ -445,9 +472,6 @@
     <t>1.5 hrs</t>
   </si>
   <si>
-    <t>Natalie - Wrote up results section of report. Still need to add scatter plots.</t>
-  </si>
-  <si>
     <t>Edited the Project Report &amp; Created Roadmap.</t>
   </si>
   <si>
@@ -458,9 +482,6 @@
   </si>
   <si>
     <t>approx. 2 hrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natalie - tidied up bits and pieces, debugging regression notebook, finalised notebooks in final branch. </t>
   </si>
   <si>
     <r>
@@ -484,7 +505,22 @@
     </r>
   </si>
   <si>
-    <t>66 hours and 37 minutes</t>
+    <t>Natalie - Wrote up results section of report.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natalie - tidied up bits and pieces, debugging regression notebook,added Lilia's bit to results bit of report, finalised notebooks in final branch. </t>
+  </si>
+  <si>
+    <t>approx 1 hr</t>
+  </si>
+  <si>
+    <t>Natalie - Submitted everything to GitHub, finalised readme file</t>
+  </si>
+  <si>
+    <t>67 hours and 37 minutes</t>
+  </si>
+  <si>
+    <t>Submitting</t>
   </si>
 </sst>
 </file>
@@ -494,7 +530,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -530,6 +566,12 @@
     </font>
     <font>
       <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -857,8 +899,8 @@
   </sheetPr>
   <dimension ref="A1:F1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1575,7 +1617,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>10</v>
       </c>
@@ -1755,7 +1797,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>10</v>
       </c>
@@ -1830,10 +1872,10 @@
         <v>18</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>10</v>
       </c>
@@ -1841,7 +1883,7 @@
         <v>45073</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>26</v>
@@ -1850,7 +1892,7 @@
         <v>11</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.15">
@@ -1861,25 +1903,37 @@
         <v>45073</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="11"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="2">
+        <v>10</v>
+      </c>
+      <c r="B54" s="10">
+        <v>45074</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2"/>
@@ -1893,10 +1947,10 @@
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F56" s="2"/>
     </row>

</xml_diff>